<commit_message>
Testing step 5 ok
</commit_message>
<xml_diff>
--- a/ancillary/plankton_elemental_quotas.xlsx
+++ b/ancillary/plankton_elemental_quotas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/ancillary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4A4E8E-176B-9344-8519-ADC0D530F56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B7B847-B3AE-4748-9AEA-C43E145A1EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1020" windowWidth="30240" windowHeight="18620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="30240" windowHeight="18620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2612" uniqueCount="1176">
   <si>
     <t>Taxon</t>
   </si>
@@ -3566,6 +3566,9 @@
   </si>
   <si>
     <t>Marine snow</t>
+  </si>
+  <si>
+    <t>Lehette, 2009</t>
   </si>
 </sst>
 </file>
@@ -3965,12 +3968,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF65"/>
+  <dimension ref="A1:AF66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="O66" sqref="O66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8300,6 +8303,35 @@
         <v>374</v>
       </c>
     </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H66">
+        <v>1.026</v>
+      </c>
+      <c r="O66" t="s">
+        <v>1175</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF62">
     <sortCondition ref="T2:T62"/>

</xml_diff>

<commit_message>
Testing with new method
</commit_message>
<xml_diff>
--- a/ancillary/plankton_elemental_quotas.xlsx
+++ b/ancillary/plankton_elemental_quotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/ancillary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C945626-EE22-6847-8C8E-D1793CA8B0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEFBC7-52D8-2F4A-83BA-37BDF4492F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32320" yWindow="-1460" windowWidth="32780" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2577" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="1179">
   <si>
     <t>Taxon</t>
   </si>
@@ -3977,12 +3977,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF64"/>
+  <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65:O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8208,6 +8208,38 @@
         <v>1173</v>
       </c>
     </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" t="s">
+        <v>96</v>
+      </c>
+      <c r="G65">
+        <v>51</v>
+      </c>
+      <c r="H65">
+        <v>1.026</v>
+      </c>
+      <c r="O65" t="s">
+        <v>1173</v>
+      </c>
+      <c r="P65" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF60">
     <sortCondition ref="T2:T60"/>

</xml_diff>

<commit_message>
Updating products with new thresholding function
</commit_message>
<xml_diff>
--- a/ancillary/plankton_elemental_quotas.xlsx
+++ b/ancillary/plankton_elemental_quotas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/ancillary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEFBC7-52D8-2F4A-83BA-37BDF4492F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357E386E-0540-2D40-BE07-3BB5489E6C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -3681,9 +3681,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3721,7 +3721,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3827,7 +3827,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3969,7 +3969,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3980,9 +3980,9 @@
   <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65:O65"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8199,7 +8199,7 @@
         <v>96</v>
       </c>
       <c r="G64">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H64">
         <v>1.026</v>
@@ -8228,7 +8228,7 @@
         <v>96</v>
       </c>
       <c r="G65">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H65">
         <v>1.026</v>

</xml_diff>